<commit_message>
feat: agregar código de limpieza de la base de datos
</commit_message>
<xml_diff>
--- a/data/DataREZUManonimos.xlsx
+++ b/data/DataREZUManonimos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milena.castromora\Documents\Próstata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://6f33fa7f78ea46e2aaca-my.sharepoint.com/personal/jose_quinterocedeno_ucr_ac_cr/Documents/Notability/Estadistica actuariall/proyecto_salud_masculina/proyecto_salud_masculina/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65B44593-BC1A-488D-A9A9-A7A052623E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{65B44593-BC1A-488D-A9A9-A7A052623E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1035B3E9-9A2D-4EC1-8B89-3B312490F8E8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario" sheetId="4" r:id="rId1"/>
@@ -1672,12 +1672,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1692,7 +1698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
@@ -1734,6 +1740,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3076,8 +3091,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1152525" y="361950"/>
-              <a:ext cx="6858000" cy="4505325"/>
+              <a:off x="1167765" y="354330"/>
+              <a:ext cx="7040880" cy="4322445"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3096,9 +3111,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="es-CR" sz="1100"/>
-                <a:t>Este gráfico no está disponible en su versión de Excel.
-Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -3159,8 +3174,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="609600" y="561975"/>
-              <a:ext cx="4572000" cy="3143250"/>
+              <a:off x="624840" y="546735"/>
+              <a:ext cx="4678680" cy="3013710"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3179,9 +3194,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="es-CR" sz="1100"/>
-                <a:t>Este gráfico no está disponible en su versión de Excel.
-Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -3194,7 +3209,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -3493,17 +3508,17 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="51.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3581,7 +3596,7 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
@@ -3635,7 +3650,7 @@
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C12" t="s">
@@ -3652,7 +3667,7 @@
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
@@ -3700,7 +3715,7 @@
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C16" t="s">
@@ -3771,7 +3786,7 @@
       <c r="A20">
         <v>11</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C20" t="s">
@@ -3788,7 +3803,7 @@
       <c r="A21">
         <v>12</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="16" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -3819,7 +3834,7 @@
       <c r="A23">
         <v>13</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="16" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -3836,7 +3851,7 @@
       <c r="A24">
         <v>14</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="16" t="s">
         <v>63</v>
       </c>
       <c r="C24" t="s">
@@ -3853,7 +3868,7 @@
       <c r="A25">
         <v>15</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="16" t="s">
         <v>65</v>
       </c>
       <c r="C25" t="s">
@@ -3870,7 +3885,7 @@
       <c r="A26">
         <v>16</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="16" t="s">
         <v>67</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -3887,7 +3902,7 @@
       <c r="A27">
         <v>17</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C27" t="s">
@@ -3916,27 +3931,27 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="11.85546875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="3"/>
+    <col min="5" max="5" width="11.88671875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="11" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="3"/>
-    <col min="12" max="13" width="12.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="3" customWidth="1"/>
-    <col min="15" max="17" width="12.7109375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="33.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="3"/>
+    <col min="12" max="13" width="12.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="3" customWidth="1"/>
+    <col min="15" max="17" width="12.6640625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="33.6640625" style="3" customWidth="1"/>
     <col min="19" max="19" width="22" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="3"/>
+    <col min="20" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="24.75">
+    <row r="1" spans="1:19">
       <c r="A1" s="14" t="s">
         <v>18</v>
       </c>
@@ -19054,7 +19069,7 @@
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19069,7 +19084,7 @@
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>